<commit_message>
Remove columns not in `EXPECTED_XLSX_COL_NAMES`
</commit_message>
<xml_diff>
--- a/plugins/polio/tests/fixtures/linelist_notification_test.xlsx
+++ b/plugins/polio/tests/fixtures/linelist_notification_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kemar/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kemar/EnCours/bluesquare/dev/iaso/plugins/polio/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B865B7-D376-9145-BE42-90F99D760F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C984B2-98BD-4F45-8790-2AC4802D32C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,6 +40,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -56,6 +57,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -72,6 +74,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -88,6 +91,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -107,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>EPID Number</t>
   </si>
@@ -188,6 +192,9 @@
   </si>
   <si>
     <t>5nt</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -198,7 +205,7 @@
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mmm&quot;-&quot;yy"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +238,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -258,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -288,11 +308,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -311,9 +346,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -327,10 +359,15 @@
     <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,7 +587,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -566,7 +603,8 @@
     <col min="9" max="9" width="25" customWidth="1"/>
     <col min="10" max="10" width="26.83203125" customWidth="1"/>
     <col min="11" max="11" width="44" customWidth="1"/>
-    <col min="12" max="13" width="23.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -606,77 +644,81 @@
       <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8"/>
+      <c r="M1" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="5">
         <v>43560</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="13"/>
-      <c r="M2" s="14"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="17" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="5">
         <v>43582</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>